<commit_message>
Set up multiple options to read from csv and excel, set up interface and read details and information to an object.
</commit_message>
<xml_diff>
--- a/src/main/resources/UserData.xlsx
+++ b/src/main/resources/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\IdeaProjects\Email_Application\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C3557A-1835-4490-973F-66D6C2AE5DF2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5701D4CB-71F9-4F49-98F9-3F20138519E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8ECF1CE4-4C12-4CD8-A92F-6865A3384E11}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="23">
   <si>
     <t>Firstname</t>
   </si>
@@ -549,7 +550,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,14 +604,17 @@
       <c r="D2" s="5">
         <v>23</v>
       </c>
-      <c r="E2" s="4">
-        <v>0</v>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -626,14 +630,17 @@
       <c r="D3" s="7">
         <v>24</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -649,14 +656,17 @@
       <c r="D4" s="5">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
-        <v>0</v>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -672,14 +682,17 @@
       <c r="D5" s="5">
         <v>26</v>
       </c>
-      <c r="E5" s="4">
-        <v>0</v>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -695,14 +708,17 @@
       <c r="D6" s="7">
         <v>29</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,14 +734,17 @@
       <c r="D7" s="5">
         <v>24</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -741,14 +760,17 @@
       <c r="D8" s="7">
         <v>21</v>
       </c>
-      <c r="E8" s="4">
-        <v>0</v>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -764,14 +786,17 @@
       <c r="D9" s="7">
         <v>26</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,14 +812,17 @@
       <c r="D10" s="5">
         <v>29</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,14 +838,17 @@
       <c r="D11" s="5">
         <v>23</v>
       </c>
-      <c r="E11" s="4">
-        <v>0</v>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -833,14 +864,17 @@
       <c r="D12" s="7">
         <v>24</v>
       </c>
-      <c r="E12" s="4">
-        <v>0</v>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,14 +890,17 @@
       <c r="D13" s="5">
         <v>28</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
+      <c r="E13" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -879,14 +916,17 @@
       <c r="D14" s="5">
         <v>26</v>
       </c>
-      <c r="E14" s="4">
-        <v>0</v>
+      <c r="E14" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,14 +942,17 @@
       <c r="D15" s="7">
         <v>29</v>
       </c>
-      <c r="E15" s="4">
-        <v>0</v>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,8 +968,8 @@
       <c r="D16" s="5">
         <v>24</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
+      <c r="E16" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>21</v>
@@ -934,8 +977,11 @@
       <c r="G16" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -948,8 +994,8 @@
       <c r="D17" s="7">
         <v>21</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
+      <c r="E17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>21</v>
@@ -957,8 +1003,11 @@
       <c r="G17" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -971,8 +1020,8 @@
       <c r="D18" s="7">
         <v>26</v>
       </c>
-      <c r="E18" s="4">
-        <v>0</v>
+      <c r="E18" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>21</v>
@@ -980,8 +1029,11 @@
       <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -994,8 +1046,8 @@
       <c r="D19" s="5">
         <v>29</v>
       </c>
-      <c r="E19" s="4">
-        <v>0</v>
+      <c r="E19" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>21</v>
@@ -1003,8 +1055,11 @@
       <c r="G19" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1017,8 +1072,8 @@
       <c r="D20" s="5">
         <v>30</v>
       </c>
-      <c r="E20" s="4">
-        <v>0</v>
+      <c r="E20" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>21</v>
@@ -1026,8 +1081,11 @@
       <c r="G20" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1040,8 +1098,8 @@
       <c r="D21" s="7">
         <v>19</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>21</v>
@@ -1049,8 +1107,11 @@
       <c r="G21" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1063,8 +1124,8 @@
       <c r="D22" s="5">
         <v>20</v>
       </c>
-      <c r="E22" s="4">
-        <v>0</v>
+      <c r="E22" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>21</v>
@@ -1072,8 +1133,11 @@
       <c r="G22" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>

</xml_diff>